<commit_message>
Update personal task document
</commit_message>
<xml_diff>
--- a/PersonalTasks/Pedja/KolonskaTabela-Pedja.xlsx
+++ b/PersonalTasks/Pedja/KolonskaTabela-Pedja.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Desktop\NoSQL\nosql-project_polyinf_2023\PersonalTasks\Pedja\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
-  <si>
-    <t>Drzava</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>Poslovni subjekat - Podaci Kompanije</t>
   </si>
@@ -44,9 +41,6 @@
     <t>Oznaka drzave</t>
   </si>
   <si>
-    <t>Naziv drzave</t>
-  </si>
-  <si>
     <t>ID kompanije</t>
   </si>
   <si>
@@ -62,40 +56,31 @@
     <t>ID projekta</t>
   </si>
   <si>
-    <t>Naziv projekta</t>
-  </si>
-  <si>
-    <t>ID Tip projekta</t>
-  </si>
-  <si>
     <t>Oznaka verzije</t>
   </si>
   <si>
-    <t>Tip verzije</t>
-  </si>
-  <si>
-    <t>Drzava verzionara</t>
-  </si>
-  <si>
     <t>Tip projekta</t>
   </si>
   <si>
-    <t>ID_TP</t>
-  </si>
-  <si>
     <t>Naziv</t>
   </si>
   <si>
     <t>Sta je predmet projekta</t>
   </si>
   <si>
-    <t>DR_Oznaka</t>
-  </si>
-  <si>
-    <t>ID_Kompanija</t>
-  </si>
-  <si>
-    <t>Projekat</t>
+    <t>Tip proizvoda</t>
+  </si>
+  <si>
+    <t>ID_projekta</t>
+  </si>
+  <si>
+    <t>Revizija</t>
+  </si>
+  <si>
+    <t>Planirani pocetak</t>
+  </si>
+  <si>
+    <t>Planirani zavrsetak</t>
   </si>
 </sst>
 </file>
@@ -124,7 +109,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -169,18 +154,54 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF66FFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -207,50 +228,13 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -259,7 +243,53 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -270,61 +300,65 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -610,144 +644,164 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.6328125" customWidth="1"/>
     <col min="2" max="2" width="14.453125" customWidth="1"/>
-    <col min="3" max="3" width="17.81640625" customWidth="1"/>
-    <col min="4" max="4" width="17.6328125" customWidth="1"/>
-    <col min="5" max="5" width="13.7265625" customWidth="1"/>
-    <col min="12" max="12" width="12.6328125" customWidth="1"/>
-    <col min="15" max="15" width="11.81640625" customWidth="1"/>
-    <col min="16" max="16" width="12.81640625" customWidth="1"/>
-    <col min="17" max="17" width="13.7265625" customWidth="1"/>
+    <col min="3" max="5" width="17.81640625" customWidth="1"/>
+    <col min="6" max="6" width="17.6328125" customWidth="1"/>
+    <col min="7" max="7" width="13.7265625" customWidth="1"/>
+    <col min="10" max="10" width="10.6328125" customWidth="1"/>
+    <col min="12" max="17" width="12.1796875" customWidth="1"/>
+    <col min="18" max="18" width="11.81640625" customWidth="1"/>
+    <col min="19" max="19" width="12.81640625" customWidth="1"/>
+    <col min="20" max="20" width="13.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="7" t="s">
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="19"/>
+      <c r="W1" s="19"/>
+      <c r="X1" s="19"/>
+    </row>
+    <row r="2" spans="1:24" ht="28" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="8" t="s">
+      <c r="R2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="N1" s="10"/>
-      <c r="O1" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="15"/>
+      <c r="S2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="W2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" ht="28" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="P2" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="R2" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="S2" s="12" t="s">
-        <v>14</v>
-      </c>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A3" s="2"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="17"/>
+      <c r="U3" s="22"/>
+      <c r="V3" s="24"/>
+      <c r="W3" s="21"/>
+      <c r="X3" s="20"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="19"/>
-      <c r="S3" s="20"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+      <c r="C4" s="11"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -764,16 +818,17 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:S1"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="C1:D1"/>
+  <mergeCells count="3">
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="I1:Q1"/>
+    <mergeCell ref="R1:X1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>